<commit_message>
Faker class,Managenews test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/LoginTestData.xlsx
+++ b/src/test/resources/LoginTestData.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\eclipse-workspace\GrocceryApplication\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85F7C8F-2464-4BA8-93EA-9DE58A9949C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{738A3E3F-725A-4CD6-A9F5-317924374250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
+    <sheet name="AdminUsersPage" sheetId="2" r:id="rId2"/>
+    <sheet name="NewsPage" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
   <si>
     <t>UserName</t>
   </si>
@@ -40,6 +42,18 @@
   </si>
   <si>
     <t>adminn</t>
+  </si>
+  <si>
+    <t>Rekha</t>
+  </si>
+  <si>
+    <t>rekha</t>
+  </si>
+  <si>
+    <t>NewsTitle</t>
+  </si>
+  <si>
+    <t>Flash Sale Alert Get 50 percent off on select groceries this weekend only</t>
   </si>
 </sst>
 </file>
@@ -359,7 +373,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -408,4 +422,58 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A7DC0C7-4E41-4253-895F-BB4591AED0D5}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6619EE2-CFF0-4FDD-B629-822A0D385B58}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>